<commit_message>
tested with dev  edition org
</commit_message>
<xml_diff>
--- a/Source/TestData.xlsx
+++ b/Source/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PlayWright-Salesforce\Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajesh.ramachandran/NewWorkspace/UIAutomationProjects/Playwright/MicrosoftPlayWright-Salesforce/Source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA840C2F-ED0D-4461-B933-7BD8AE8EC01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB427D3-F6C6-824E-A78B-0E0624EA72A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A2815E69-8986-364A-9557-36816B6FF178}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{A2815E69-8986-364A-9557-36816B6FF178}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
   <si>
     <t>Url</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>RecordType</t>
-  </si>
-  <si>
     <t>Billing Country</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>ravi0389@gmail.com</t>
   </si>
   <si>
-    <t>Services</t>
-  </si>
-  <si>
     <t>Automated Account - Microsoft PlayWright</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Sales Contact</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -192,9 +183,6 @@
     <t>Web</t>
   </si>
   <si>
-    <t>Marketing Process</t>
-  </si>
-  <si>
     <t>Test Opportunity - Automation by PlayWright</t>
   </si>
   <si>
@@ -222,26 +210,34 @@
     <t>8/31/2021</t>
   </si>
   <si>
-    <t>ORGURL</t>
-  </si>
-  <si>
-    <t>USERNAME</t>
-  </si>
-  <si>
-    <t>PWD</t>
-  </si>
-  <si>
-    <t>TOKEN</t>
+    <t>https://rajeshlwc-dev-ed.my.salesforce.com</t>
+  </si>
+  <si>
+    <t>rajesh.lwc@sfdcinfy.com</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>2ss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,10 +292,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -310,8 +307,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -627,10 +626,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
@@ -638,7 +637,7 @@
     <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -649,43 +648,47 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{07377DEA-5D65-E54E-A365-12AA8A0512D2}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{D06DF668-4663-EF47-8CC6-6710BF05C6FB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5202B449-7F0E-184B-841A-6BF4DCEDC67D}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -693,100 +696,92 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="4" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -797,122 +792,114 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941BE292-14FD-D147-85A7-CE1E412C580E}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="45.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <f>Account!B2</f>
+        <v>Automated Account - Microsoft PlayWright</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="str">
-        <f>Account!B3</f>
-        <v>Automated Account - Microsoft PlayWright</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="4" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -922,97 +909,89 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C259D5ED-9AEA-C64F-A44B-AA3BC565DECB}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <f>Account!B2</f>
+        <v>Automated Account - Microsoft PlayWright</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="str">
-        <f>Account!B3</f>
-        <v>Automated Account - Microsoft PlayWright</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="B7" s="2">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="2">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>